<commit_message>
Auto-committed on 2021/12/07 週二
Former-commit-id: b3060be5393f870fc883fa5cadcfaa7e86447b8a
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanBorTx.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanBorTx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L3-帳務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D34654-F0C7-4B6F-8450-1BF663AEE5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7289D98E-07E7-4073-89AB-612016CACB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="328">
   <si>
     <t>備註說明</t>
   </si>
@@ -1337,6 +1337,13 @@
   </si>
   <si>
     <t>CustNo = ,AND FacmNo = ,AND BormNo &gt;= ,AND BormNo &lt;= ,AND IntEndDate = ,AND TitaHCode ^i ,AND AcDate = ,AND TitaTlrNo = ,AND TitaTxtNo =</t>
+  </si>
+  <si>
+    <t>borxEntryDateDescRange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AcDate DESC ,TitaKinBr asc ,TitaTlrNo asc ,TitaTxtNo DESC</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2075,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -3222,9 +3229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3373,7 +3380,15 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="C14" s="37"/>
+      <c r="A14" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>327</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3386,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>

</xml_diff>